<commit_message>
rajout titre page accueil et keywords page2
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Documents Guylaine\projet4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48838914-C071-4674-B63F-68D5E111C91E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F760BF-D7E8-4C73-83AA-C261B9B2FF60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="6930" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Catégorie</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>temps de chargement nul</t>
-  </si>
-  <si>
-    <t>Manifier et compresser les ressources (images et code)</t>
   </si>
   <si>
     <r>
@@ -177,6 +174,18 @@
   </si>
   <si>
     <t>Ajouter une méta-description sur chacune des pages</t>
+  </si>
+  <si>
+    <t>Langue</t>
+  </si>
+  <si>
+    <t>Les documents html ont comme paramètre de langue "Default"</t>
+  </si>
+  <si>
+    <t>Changer ce paramètre pour mettre "fr" à la place</t>
+  </si>
+  <si>
+    <t>Magnifier et compresser les ressources (images et code)</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -653,13 +662,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>0</v>
@@ -695,10 +704,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E12" s="4" t="b">
         <v>0</v>
@@ -715,16 +724,16 @@
     </row>
     <row r="16" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
@@ -735,13 +744,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -752,13 +761,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
@@ -769,19 +778,35 @@
         <v>13</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>